<commit_message>
Conversion to total flow and to intervening
</commit_message>
<xml_diff>
--- a/multimodel-disag/data/nf-intervening-total-conversion.xlsx
+++ b/multimodel-disag/data/nf-intervening-total-conversion.xlsx
@@ -6480,7 +6480,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="V22" sqref="C3:V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7981,6 +7981,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7994,7 +7995,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B2" sqref="B2:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8203,10 +8204,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -8484,10 +8485,10 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -9495,6 +9496,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>